<commit_message>
filling marker info into status 8
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_1800.xlsx
+++ b/bioSample/bioSample_1800.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="47">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">CNAG_00841.CNAG_06339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDY2188</t>
   </si>
   <si>
     <t xml:space="preserve">CNAG_06327</t>
@@ -256,8 +259,8 @@
   </sheetPr>
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47:E52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L50" activeCellId="0" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1797,8 +1800,11 @@
       <c r="D47" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="E47" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="F47" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>16</v>
@@ -1809,6 +1815,9 @@
       <c r="I47" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="J47" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
@@ -1823,8 +1832,11 @@
       <c r="D48" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="E48" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="F48" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>16</v>
@@ -1835,6 +1847,9 @@
       <c r="I48" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="J48" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -1849,8 +1864,11 @@
       <c r="D49" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="E49" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="F49" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>16</v>
@@ -1861,6 +1879,9 @@
       <c r="I49" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="J49" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -1876,7 +1897,7 @@
         <v>13</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>16</v>
@@ -1887,6 +1908,9 @@
       <c r="I50" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="J50" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
@@ -1902,7 +1926,7 @@
         <v>13</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>16</v>
@@ -1913,6 +1937,9 @@
       <c r="I51" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="J51" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
@@ -1928,7 +1955,7 @@
         <v>13</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G52" s="0" t="s">
         <v>16</v>
@@ -1938,6 +1965,9 @@
       </c>
       <c r="I52" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>